<commit_message>
Put some bugs on hold
Removing chips throws Exception
</commit_message>
<xml_diff>
--- a/Outputs/stat averages.xlsx
+++ b/Outputs/stat averages.xlsx
@@ -260,16 +260,16 @@
                 <formatCode>0.0%</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>0.6977407019381875</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.4273166268894192</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>0.6935916552667577</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>0.4247692716640085</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -338,16 +338,16 @@
                 <formatCode>0.0%</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>0.02199423782084861</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.2370628480509149</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>0.4122879616963065</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>0.05547687400318978</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -416,16 +416,16 @@
                 <formatCode>0.0%</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>0.00366663174436878</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.03262330946698486</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>0.04446169630642956</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>0.006923817118553958</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -690,16 +690,16 @@
                 <formatCode>General</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>8</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>71</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>20</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>11</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -787,16 +787,16 @@
                 <formatCode>General</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>25</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>148</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>39</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>22</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -1085,16 +1085,16 @@
                 <formatCode>General</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>1021</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>348</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>780</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>725</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -1283,29 +1283,6 @@
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
-      <txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1800" b="1" i="0" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:r>
-            <a:t>None</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </txPr>
     </title>
     <plotArea>
       <layout/>
@@ -1399,16 +1376,16 @@
                 <formatCode>0.0%</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>0.5334857982370225</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.3398132183908046</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>0.5516551282051284</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>0.426671724137931</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -1636,16 +1613,16 @@
                 <formatCode>0.0%</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>0.7293474402730376</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.4834236760124611</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>0.694919714540589</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>0.4766204911742133</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -1714,16 +1691,16 @@
                 <formatCode>0.0%</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>0.0237358361774744</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.2972548286604362</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>0.3541101694915254</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>0.05375287797390637</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -1792,16 +1769,16 @@
                 <formatCode>0.0%</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>0.005801160409556313</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.03801090342679129</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>0.03479768064228368</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>0.00690230237912509</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -2094,16 +2071,16 @@
                 <formatCode>0.00</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>0.244681103337609</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>1.796713943224349</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>2.366905220161249</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>0.4605772959808836</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -2370,16 +2347,16 @@
                 <formatCode>0.0%</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>0.2850150170648466</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.1556093457943925</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>0.2215887600356823</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>0.1826277820414429</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -2469,16 +2446,16 @@
                 <formatCode>0.0%</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>0.1538648464163821</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.06362367601246106</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>0.1076052631578948</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>0.08861972371450498</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -2744,16 +2721,16 @@
                 <formatCode>General</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>25</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>212</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>311</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>46</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -2841,16 +2818,16 @@
                 <formatCode>General</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>59</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>492</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>538</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>110</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -3147,16 +3124,16 @@
                 <formatCode>General</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>2930</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>1605</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>2242</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>2606</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -3345,29 +3322,6 @@
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
-      <txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1800" b="1" i="0" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:r>
-            <a:t>None</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </txPr>
     </title>
     <plotArea>
       <layout/>
@@ -3461,16 +3415,16 @@
                 <formatCode>0.0%</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>0.5389436860068259</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.4274641744548284</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>0.4937872435325601</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>0.5037041442824253</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -3756,16 +3710,16 @@
                 <formatCode>0.00</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>0.225520266065722</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>1.615846900381764</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>3.089958663338651</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>0.4674519850438521</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -4032,16 +3986,16 @@
                 <formatCode>0.0%</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>0.2561629125196437</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.1439729514717581</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>0.212686730506156</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>0.1525699096225413</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -4131,16 +4085,16 @@
                 <formatCode>0.0%</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>0.1398768988999476</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.06054335719968178</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>0.09564090287277704</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>0.07853960659223817</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -4406,16 +4360,16 @@
                 <formatCode>General</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>17</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>146</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>284</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>25</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -4503,16 +4457,16 @@
                 <formatCode>General</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>35</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>353</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>484</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>56</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -4801,16 +4755,16 @@
                 <formatCode>General</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>1909</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>1257</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>1462</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>1881</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -4999,29 +4953,6 @@
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
-      <txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1800" b="1" i="0" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:r>
-            <a:t>None</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </txPr>
     </title>
     <plotArea>
       <layout/>
@@ -5126,16 +5057,16 @@
                 <formatCode>0.0%</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>0.5314876898899947</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.410988862370724</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>0.4468994528043774</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>0.5104885699096225</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -5363,16 +5294,16 @@
                 <formatCode>0.0%</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>0.7864103819784523</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.6838390804597702</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>0.697470512820513</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>0.6110648275862069</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -5441,16 +5372,16 @@
                 <formatCode>0.0%</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>0.02728501469147893</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.5116293103448276</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>0.2461217948717949</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>0.04959172413793104</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -5519,16 +5450,16 @@
                 <formatCode>0.0%</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>0.009785602350636623</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.05459166666666667</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>0.01795884615384616</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>0.006891448275862072</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -5832,16 +5763,16 @@
                 <formatCode>0.00</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>0.2939985925832188</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>2.336307330297411</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>0.7831644753010567</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>0.4617729046541815</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -6108,16 +6039,16 @@
                 <formatCode>0.0%</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>0.339001958863859</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.1927327586206896</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>0.2384794871794874</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>0.2605006896551726</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -6207,16 +6138,16 @@
                 <formatCode>0.0%</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>0.1802859941234085</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.07469540229885058</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="2">
-                  <v>0.1297179487179488</v>
+                  <v>0</v>
                 </pt>
                 <pt idx="3">
-                  <v>0.1146882758620689</v>
+                  <v>0</v>
                 </pt>
               </numCache>
             </numRef>
@@ -7160,8 +7091,8 @@
   </sheetPr>
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="I51" sqref="I51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A17:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -7263,7 +7194,7 @@
         <v>0.02101451451451451</v>
       </c>
       <c r="E2" s="6" t="n">
-        <v>0.003503303303303304</v>
+        <v>0.002506356356356356</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>0.1307057057057058</v>
@@ -7275,7 +7206,7 @@
         <v>0.1386351351351351</v>
       </c>
       <c r="I2" s="6" t="n">
-        <v>0.5312432432432432</v>
+        <v>0.5405085085085085</v>
       </c>
       <c r="J2" s="6" t="n">
         <v>0.4857142857142857</v>
@@ -7306,7 +7237,7 @@
         <v>0.239624025974026</v>
       </c>
       <c r="E3" s="6" t="n">
-        <v>0.04285480519480517</v>
+        <v>0.01948090909090908</v>
       </c>
       <c r="F3" s="6" t="n">
         <v>0.3373668831168831</v>
@@ -7318,7 +7249,7 @@
         <v>0.06301623376623376</v>
       </c>
       <c r="I3" s="6" t="n">
-        <v>0.4370857142857143</v>
+        <v>0.4559844155844156</v>
       </c>
       <c r="J3" s="6" t="n">
         <v>0.4004683840749415</v>
@@ -7349,7 +7280,7 @@
         <v>0.3873008083140878</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>0.04792840646651271</v>
+        <v>0.01673152424942263</v>
       </c>
       <c r="F4" s="6" t="n">
         <v>0.5510814087759814</v>
@@ -7361,7 +7292,7 @@
         <v>0.08883775981524253</v>
       </c>
       <c r="I4" s="6" t="n">
-        <v>0.4280525404157042</v>
+        <v>0.4437938799076212</v>
       </c>
       <c r="J4" s="6" t="n">
         <v>0.5795454545454546</v>
@@ -7393,7 +7324,7 @@
         <v>0.0492467289719626</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>0.006085841121495325</v>
+        <v>0.003740841121495326</v>
       </c>
       <c r="F5" s="6" t="n">
         <v>0.1955275700934578</v>
@@ -7405,7 +7336,7 @@
         <v>0.08307336448598131</v>
       </c>
       <c r="I5" s="6" t="n">
-        <v>0.5227742990654205</v>
+        <v>0.5349238317757009</v>
       </c>
       <c r="J5" s="6" t="n">
         <v>0.4655172413793103</v>
@@ -7575,8 +7506,8 @@
   </sheetPr>
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N5" sqref="C2:N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -7682,13 +7613,13 @@
         </is>
       </c>
       <c r="C2" s="6" t="n">
-        <v>0.7864103819784523</v>
+        <v>0.7883692458374142</v>
       </c>
       <c r="D2" s="6" t="n">
         <v>0.02728501469147893</v>
       </c>
       <c r="E2" s="6" t="n">
-        <v>0.009785602350636623</v>
+        <v>0.008801273261508322</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>0.1892154750244857</v>
@@ -7727,25 +7658,25 @@
         </is>
       </c>
       <c r="C3" s="6" t="n">
-        <v>0.6838390804597702</v>
+        <v>0.686712643678161</v>
       </c>
       <c r="D3" s="6" t="n">
-        <v>0.5116293103448276</v>
+        <v>0.5145028735632184</v>
       </c>
       <c r="E3" s="6" t="n">
-        <v>0.05459166666666667</v>
+        <v>0.03161091954022989</v>
       </c>
       <c r="F3" s="6" t="n">
         <v>0.5592040229885059</v>
       </c>
       <c r="G3" s="6" t="n">
-        <v>0.1927327586206896</v>
+        <v>0.1984798850574713</v>
       </c>
       <c r="H3" s="6" t="n">
         <v>0.07469540229885058</v>
       </c>
       <c r="I3" s="6" t="n">
-        <v>0.3398132183908046</v>
+        <v>0.3642385057471265</v>
       </c>
       <c r="J3" s="6" t="n">
         <v>0.4797297297297297</v>
@@ -7778,7 +7709,7 @@
         <v>0.2461217948717949</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>0.01795884615384616</v>
+        <v>0.006422948717948717</v>
       </c>
       <c r="F4" s="6" t="n">
         <v>0.4680371794871796</v>
@@ -7790,7 +7721,7 @@
         <v>0.1297179487179488</v>
       </c>
       <c r="I4" s="6" t="n">
-        <v>0.5516551282051284</v>
+        <v>0.554219230769231</v>
       </c>
       <c r="J4" s="6" t="n">
         <v>0.5128205128205128</v>
@@ -7834,7 +7765,7 @@
         <v>0.1146882758620689</v>
       </c>
       <c r="I5" s="6" t="n">
-        <v>0.426671724137931</v>
+        <v>0.4514993103448275</v>
       </c>
       <c r="J5" s="6" t="n">
         <v>0.5</v>
@@ -7986,10 +7917,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P43"/>
+  <dimension ref="A1:P80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -8096,7 +8027,7 @@
         <v>0.02303610467042067</v>
       </c>
       <c r="E2" s="6" t="n">
-        <v>0.005630142431268631</v>
+        <v>0.004632991056641274</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>0.1505869493209673</v>
@@ -8139,7 +8070,7 @@
         <v>0.2903215042372882</v>
       </c>
       <c r="E3" s="6" t="n">
-        <v>0.04554894067796611</v>
+        <v>0.02171530720338985</v>
       </c>
       <c r="F3" s="6" t="n">
         <v>0.3824841101694917</v>
@@ -8182,7 +8113,7 @@
         <v>0.3431349522292994</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>0.0382266719745223</v>
+        <v>0.01353049363057325</v>
       </c>
       <c r="F4" s="6" t="n">
         <v>0.5260991242038218</v>
@@ -8225,7 +8156,7 @@
         <v>0.04925514834205934</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>0.006278324607329838</v>
+        <v>0.004531343804537522</v>
       </c>
       <c r="F5" s="6" t="n">
         <v>0.2164701570680628</v>
@@ -8255,141 +8186,141 @@
         <v>2865</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
+    <row r="61">
+      <c r="A61" t="inlineStr">
         <is>
           <t>040921</t>
         </is>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
+    <row r="62">
+      <c r="A62" t="inlineStr">
         <is>
           <t>041621</t>
         </is>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
+    <row r="63">
+      <c r="A63" t="inlineStr">
         <is>
           <t>041921</t>
         </is>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
+    <row r="64">
+      <c r="A64" t="inlineStr">
         <is>
           <t>042421</t>
         </is>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
+    <row r="65">
+      <c r="A65" t="inlineStr">
         <is>
           <t>042621</t>
         </is>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
+    <row r="66">
+      <c r="A66" t="inlineStr">
         <is>
           <t>042921</t>
         </is>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
+    <row r="67">
+      <c r="A67" t="inlineStr">
         <is>
           <t>050421</t>
         </is>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
+    <row r="68">
+      <c r="A68" t="inlineStr">
         <is>
           <t>051321</t>
         </is>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
+    <row r="69">
+      <c r="A69" t="inlineStr">
         <is>
           <t>051721</t>
         </is>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
+    <row r="70">
+      <c r="A70" t="inlineStr">
         <is>
           <t>052021</t>
         </is>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
+    <row r="71">
+      <c r="A71" t="inlineStr">
         <is>
           <t>052421</t>
         </is>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
+    <row r="72">
+      <c r="A72" t="inlineStr">
         <is>
           <t>052721</t>
         </is>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
+    <row r="73">
+      <c r="A73" t="inlineStr">
         <is>
           <t>052821</t>
         </is>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
+    <row r="74">
+      <c r="A74" t="inlineStr">
         <is>
           <t>053121</t>
         </is>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
+    <row r="75">
+      <c r="A75" t="inlineStr">
         <is>
           <t>060721</t>
         </is>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
+    <row r="76">
+      <c r="A76" t="inlineStr">
         <is>
           <t>061021</t>
         </is>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
+    <row r="77">
+      <c r="A77" t="inlineStr">
         <is>
           <t>061421</t>
         </is>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
+    <row r="78">
+      <c r="A78" t="inlineStr">
         <is>
           <t>061521</t>
         </is>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
+    <row r="79">
+      <c r="A79" t="inlineStr">
         <is>
           <t>061721</t>
         </is>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
+    <row r="80">
+      <c r="A80" t="inlineStr">
         <is>
           <t>062121</t>
         </is>

</xml_diff>